<commit_message>
Agregué artículo sometido Andrés
</commit_message>
<xml_diff>
--- a/data/supervision_pre_en.xlsx
+++ b/data/supervision_pre_en.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\Grants\Datos CV\archivos (1)\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GitHub\Mile_CV\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C0C4B6-88B1-46C8-AFDC-BD50D563EA6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9EFF0E6-03DD-4160-AB09-28532B95AEDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="50">
   <si>
     <t>what</t>
   </si>
@@ -178,6 +178,12 @@
   </si>
   <si>
     <t>Research project: \textit{Relación entre el nivel de consumo de alcohol y el rendimiento en procesos de función ejecutiva en estudiantes universitarios entre los 18 y 25 años [Relationship between the level of alcohol consumption and performance in executive function processes in university students between 18 and 25 years of age]}</t>
+  </si>
+  <si>
+    <t>Angela Rivero Valderrama \&amp; Sebastián Camilo Valenzuela</t>
+  </si>
+  <si>
+    <t>Research project: \textit{Preferencias por estímulos sexuales eróticos según género y la orientación sexual: un estudio con eye-tracking[Preferences for erotic sexual stimuli according to gender and sexual orientation: a study with eye-tracking]}</t>
   </si>
 </sst>
 </file>
@@ -1030,10 +1036,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="58.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1062,7 +1068,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -1070,13 +1076,13 @@
         <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -1084,50 +1090,50 @@
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -1135,18 +1141,17 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="2"/>
+        <v>32</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -1156,13 +1161,13 @@
         <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -1174,50 +1179,51 @@
         <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -1225,16 +1231,16 @@
         <v>5</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -1242,13 +1248,13 @@
         <v>5</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -1256,53 +1262,53 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2" t="s">
+    <row r="15" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
@@ -1310,12 +1316,29 @@
         <v>24</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E16" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>